<commit_message>
Pvalue between treatment arms
</commit_message>
<xml_diff>
--- a/Notebooks/Test.xlsx
+++ b/Notebooks/Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Cohort</t>
   </si>
@@ -28,19 +28,58 @@
     <t>Fold 1</t>
   </si>
   <si>
+    <t>Fold 2</t>
+  </si>
+  <si>
+    <t>Fold 3</t>
+  </si>
+  <si>
+    <t>Fold 4</t>
+  </si>
+  <si>
+    <t>Fold 5</t>
+  </si>
+  <si>
+    <t>Fold 6</t>
+  </si>
+  <si>
+    <t>Fold 7</t>
+  </si>
+  <si>
+    <t>Fold 8</t>
+  </si>
+  <si>
+    <t>Fold 9</t>
+  </si>
+  <si>
     <t>Cohort A</t>
   </si>
   <si>
-    <t>Type A</t>
+    <t>['Type A']</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Type B</t>
+    <t>['Type B']</t>
+  </si>
+  <si>
+    <t>['Type C']</t>
+  </si>
+  <si>
+    <t>['Type D']</t>
+  </si>
+  <si>
+    <t>['Type E']</t>
   </si>
   <si>
     <t>Cohort B</t>
+  </si>
+  <si>
+    <t>P-value (avelumab + axitinib vs sunitinib)</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -64,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,6 +113,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE4B2B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -90,9 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,13 +433,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,55 +452,421 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>-1.779255998560584</v>
+      </c>
+      <c r="E2">
+        <v>-0.04510315045938534</v>
+      </c>
+      <c r="F2">
+        <v>2.465123354259019</v>
+      </c>
+      <c r="G2">
+        <v>0.1526151866546164</v>
+      </c>
+      <c r="H2">
+        <v>-1.0179149943903</v>
+      </c>
+      <c r="I2">
+        <v>-1.303240683302661</v>
+      </c>
+      <c r="J2">
+        <v>-1.377819114698333</v>
+      </c>
+      <c r="K2">
+        <v>-0.7122052321026323</v>
+      </c>
+      <c r="L2">
+        <v>-1.530987964169075</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>1.647889664030219</v>
+        <v>-0.7195217567555066</v>
       </c>
       <c r="D3">
-        <v>0.3244558121291163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>-0.1169508558564924</v>
+      </c>
+      <c r="E3">
+        <v>-1.073786449218701</v>
+      </c>
+      <c r="F3">
+        <v>0.7227664053757503</v>
+      </c>
+      <c r="G3">
+        <v>-1.369186971243697</v>
+      </c>
+      <c r="H3">
+        <v>-1.736043066679239</v>
+      </c>
+      <c r="I3">
+        <v>-1.33719832833978</v>
+      </c>
+      <c r="J3">
+        <v>1.446830432624888</v>
+      </c>
+      <c r="K3">
+        <v>-1.433352777861467</v>
+      </c>
+      <c r="L3">
+        <v>-0.8720857571204663</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.5602825673208243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>0.05813590100630157</v>
+        <v>-0.1573317846041827</v>
       </c>
       <c r="D4">
-        <v>0.6945825438303127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>1.079755508515075</v>
+      </c>
+      <c r="E4">
+        <v>0.1886145646516095</v>
+      </c>
+      <c r="F4">
+        <v>0.1478142601639852</v>
+      </c>
+      <c r="G4">
+        <v>0.3056050045085065</v>
+      </c>
+      <c r="H4">
+        <v>0.9694042701470049</v>
+      </c>
+      <c r="I4">
+        <v>-0.8046288719735758</v>
+      </c>
+      <c r="J4">
+        <v>0.8578259353940139</v>
+      </c>
+      <c r="K4">
+        <v>-0.4403974426606984</v>
+      </c>
+      <c r="L4">
+        <v>-1.694521545296632</v>
+      </c>
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.8869270417806654</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>0.8681876971315023</v>
+        <v>-1.153689983868636</v>
       </c>
       <c r="D5">
-        <v>-0.5870141792344868</v>
+        <v>1.763645932041266</v>
+      </c>
+      <c r="E5">
+        <v>-0.05881116575516901</v>
+      </c>
+      <c r="F5">
+        <v>-0.5015252233096519</v>
+      </c>
+      <c r="G5">
+        <v>0.8718153098583075</v>
+      </c>
+      <c r="H5">
+        <v>-0.09984318861983975</v>
+      </c>
+      <c r="I5">
+        <v>-0.06643497319662964</v>
+      </c>
+      <c r="J5">
+        <v>-1.499679143695234</v>
+      </c>
+      <c r="K5">
+        <v>0.4954971715508118</v>
+      </c>
+      <c r="L5">
+        <v>1.762850193890608</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.831204094653385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>0.6539467453348656</v>
+      </c>
+      <c r="D6">
+        <v>-2.03912041229015</v>
+      </c>
+      <c r="E6">
+        <v>-1.416424090103757</v>
+      </c>
+      <c r="F6">
+        <v>-0.8207594410985131</v>
+      </c>
+      <c r="G6">
+        <v>0.9474883257687298</v>
+      </c>
+      <c r="H6">
+        <v>0.2285461551269918</v>
+      </c>
+      <c r="I6">
+        <v>-0.4600668650411009</v>
+      </c>
+      <c r="J6">
+        <v>1.157006329810376</v>
+      </c>
+      <c r="K6">
+        <v>-0.6234614139680424</v>
+      </c>
+      <c r="L6">
+        <v>-0.9345640742362571</v>
+      </c>
+      <c r="O6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.9336656249530835</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>-0.9131912133187131</v>
+      </c>
+      <c r="D7">
+        <v>0.5009210561639066</v>
+      </c>
+      <c r="E7">
+        <v>-0.7362381103858457</v>
+      </c>
+      <c r="F7">
+        <v>0.8314261594125762</v>
+      </c>
+      <c r="G7">
+        <v>0.7476315138500816</v>
+      </c>
+      <c r="H7">
+        <v>-1.326780920022784</v>
+      </c>
+      <c r="I7">
+        <v>1.2526984969859</v>
+      </c>
+      <c r="J7">
+        <v>1.083676486434104</v>
+      </c>
+      <c r="K7">
+        <v>1.352680414362624</v>
+      </c>
+      <c r="L7">
+        <v>-0.6645792070954761</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>-1.07396043247548</v>
+      </c>
+      <c r="D8">
+        <v>-0.8942166489552742</v>
+      </c>
+      <c r="E8">
+        <v>-1.719010718111805</v>
+      </c>
+      <c r="F8">
+        <v>1.114682160967344</v>
+      </c>
+      <c r="G8">
+        <v>1.309405557362332</v>
+      </c>
+      <c r="H8">
+        <v>-0.06852066420982282</v>
+      </c>
+      <c r="I8">
+        <v>-3.327330153434886</v>
+      </c>
+      <c r="J8">
+        <v>1.387570548311583</v>
+      </c>
+      <c r="K8">
+        <v>-0.3978080697452196</v>
+      </c>
+      <c r="L8">
+        <v>0.6091082670346301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0.7248848294437311</v>
+      </c>
+      <c r="D9">
+        <v>-0.2443523127781745</v>
+      </c>
+      <c r="E9">
+        <v>-0.1926569900464277</v>
+      </c>
+      <c r="F9">
+        <v>-0.4740428635829493</v>
+      </c>
+      <c r="G9">
+        <v>-0.2555324690860644</v>
+      </c>
+      <c r="H9">
+        <v>1.441002416463198</v>
+      </c>
+      <c r="I9">
+        <v>-0.8655766539731472</v>
+      </c>
+      <c r="J9">
+        <v>-1.261245091178943</v>
+      </c>
+      <c r="K9">
+        <v>0.7173118016479986</v>
+      </c>
+      <c r="L9">
+        <v>0.3215327825064397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>1.095610546883083</v>
+      </c>
+      <c r="D10">
+        <v>1.034153101808478</v>
+      </c>
+      <c r="E10">
+        <v>-0.9461047209673817</v>
+      </c>
+      <c r="F10">
+        <v>-1.368948450677739</v>
+      </c>
+      <c r="G10">
+        <v>1.550305204396043</v>
+      </c>
+      <c r="H10">
+        <v>-0.8989445919606539</v>
+      </c>
+      <c r="I10">
+        <v>-1.670579346817776</v>
+      </c>
+      <c r="J10">
+        <v>1.240009283434738</v>
+      </c>
+      <c r="K10">
+        <v>1.193213256954198</v>
+      </c>
+      <c r="L10">
+        <v>-0.8680770822312189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>-0.2567707288198824</v>
+      </c>
+      <c r="D11">
+        <v>-0.6727435509920217</v>
+      </c>
+      <c r="E11">
+        <v>-1.226255849787006</v>
+      </c>
+      <c r="F11">
+        <v>-0.6539774842465743</v>
+      </c>
+      <c r="G11">
+        <v>-0.3420152463784832</v>
+      </c>
+      <c r="H11">
+        <v>0.4917744454399575</v>
+      </c>
+      <c r="I11">
+        <v>-0.2437963395075148</v>
+      </c>
+      <c r="J11">
+        <v>-0.08928021392893951</v>
+      </c>
+      <c r="K11">
+        <v>0.5555691979759015</v>
+      </c>
+      <c r="L11">
+        <v>-0.5549574785070762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>